<commit_message>
#29 Update ADPPK spec for xportr 0.3.0
</commit_message>
<xml_diff>
--- a/content/data/adpc/ADPPK_spec_text.xlsx
+++ b/content/data/adpc/ADPPK_spec_text.xlsx
@@ -5,22 +5,25 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dickinsj\OneDrive - Navitas Life Sciences\ADPPK\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\__transfer\admiral_test\end_to_end_examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:40009_{A73C868D-8D7A-4BBD-A69F-DCCBEA596C73}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{096425F1-DBB5-455A-9213-1D171FD94F76}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C6102E-6530-426A-8D22-763C1C0F7862}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19008" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19005" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ADPPK" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ADPPK!$A$1:$G$83</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="176">
   <si>
     <t>Variable Name</t>
   </si>
@@ -539,6 +542,15 @@
   </si>
   <si>
     <t>Baseline Alanine transaminase</t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>Length</t>
   </si>
 </sst>
 </file>
@@ -1380,21 +1392,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D83"/>
+  <dimension ref="A1:G83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1407,8 +1422,17 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1421,8 +1445,14 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>100</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1435,8 +1465,14 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1449,8 +1485,14 @@
       <c r="D4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>21</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1463,8 +1505,14 @@
       <c r="D5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>8</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1477,8 +1525,14 @@
       <c r="D6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <v>8</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1491,8 +1545,14 @@
       <c r="D7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>8</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1505,8 +1565,14 @@
       <c r="D8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <v>100</v>
+      </c>
+      <c r="G8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1519,8 +1585,14 @@
       <c r="D9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <v>30</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -1533,8 +1605,14 @@
       <c r="D10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <v>8</v>
+      </c>
+      <c r="G10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1547,8 +1625,14 @@
       <c r="D11" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <v>8</v>
+      </c>
+      <c r="G11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1561,8 +1645,14 @@
       <c r="D12" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12">
+        <v>8</v>
+      </c>
+      <c r="G12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -1575,8 +1665,14 @@
       <c r="D13" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E13">
+        <v>8</v>
+      </c>
+      <c r="G13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -1589,8 +1685,14 @@
       <c r="D14" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E14">
+        <v>8</v>
+      </c>
+      <c r="G14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -1603,8 +1705,14 @@
       <c r="D15" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E15">
+        <v>8</v>
+      </c>
+      <c r="G15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -1617,8 +1725,14 @@
       <c r="D16" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16">
+        <v>8</v>
+      </c>
+      <c r="G16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -1631,8 +1745,14 @@
       <c r="D17" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17">
+        <v>8</v>
+      </c>
+      <c r="G17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -1645,8 +1765,14 @@
       <c r="D18" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18">
+        <v>8</v>
+      </c>
+      <c r="G18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -1659,8 +1785,14 @@
       <c r="D19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19">
+        <v>8</v>
+      </c>
+      <c r="G19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>45</v>
       </c>
@@ -1673,8 +1805,14 @@
       <c r="D20" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E20">
+        <v>8</v>
+      </c>
+      <c r="G20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>47</v>
       </c>
@@ -1687,8 +1825,14 @@
       <c r="D21" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E21">
+        <v>8</v>
+      </c>
+      <c r="G21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>49</v>
       </c>
@@ -1701,8 +1845,14 @@
       <c r="D22" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E22">
+        <v>8</v>
+      </c>
+      <c r="G22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -1715,8 +1865,14 @@
       <c r="D23" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E23">
+        <v>200</v>
+      </c>
+      <c r="G23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>53</v>
       </c>
@@ -1729,8 +1885,14 @@
       <c r="D24" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E24">
+        <v>8</v>
+      </c>
+      <c r="G24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>55</v>
       </c>
@@ -1743,8 +1905,14 @@
       <c r="D25" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E25">
+        <v>200</v>
+      </c>
+      <c r="G25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>57</v>
       </c>
@@ -1757,8 +1925,14 @@
       <c r="D26" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E26">
+        <v>8</v>
+      </c>
+      <c r="G26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>59</v>
       </c>
@@ -1771,8 +1945,14 @@
       <c r="D27" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E27">
+        <v>40</v>
+      </c>
+      <c r="G27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>61</v>
       </c>
@@ -1785,8 +1965,14 @@
       <c r="D28" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E28">
+        <v>8</v>
+      </c>
+      <c r="G28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>63</v>
       </c>
@@ -1799,8 +1985,14 @@
       <c r="D29" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E29">
+        <v>8</v>
+      </c>
+      <c r="G29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>65</v>
       </c>
@@ -1813,8 +2005,14 @@
       <c r="D30" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E30">
+        <v>8</v>
+      </c>
+      <c r="G30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>67</v>
       </c>
@@ -1827,8 +2025,14 @@
       <c r="D31" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E31">
+        <v>8</v>
+      </c>
+      <c r="G31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>69</v>
       </c>
@@ -1841,8 +2045,14 @@
       <c r="D32" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E32">
+        <v>10</v>
+      </c>
+      <c r="G32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>71</v>
       </c>
@@ -1855,8 +2065,14 @@
       <c r="D33" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E33">
+        <v>200</v>
+      </c>
+      <c r="G33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>73</v>
       </c>
@@ -1869,8 +2085,14 @@
       <c r="D34" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E34">
+        <v>8</v>
+      </c>
+      <c r="G34">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>75</v>
       </c>
@@ -1883,8 +2105,14 @@
       <c r="D35" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E35">
+        <v>8</v>
+      </c>
+      <c r="G35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>77</v>
       </c>
@@ -1897,8 +2125,14 @@
       <c r="D36" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E36">
+        <v>8</v>
+      </c>
+      <c r="G36">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>79</v>
       </c>
@@ -1911,8 +2145,14 @@
       <c r="D37" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="G37">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>81</v>
       </c>
@@ -1925,8 +2165,14 @@
       <c r="D38" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E38">
+        <v>8</v>
+      </c>
+      <c r="G38">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>83</v>
       </c>
@@ -1939,8 +2185,14 @@
       <c r="D39" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="G39">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>85</v>
       </c>
@@ -1953,8 +2205,14 @@
       <c r="D40" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E40">
+        <v>8</v>
+      </c>
+      <c r="G40">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>87</v>
       </c>
@@ -1967,8 +2225,14 @@
       <c r="D41" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E41">
+        <v>8</v>
+      </c>
+      <c r="G41">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>89</v>
       </c>
@@ -1981,8 +2245,14 @@
       <c r="D42" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E42">
+        <v>8</v>
+      </c>
+      <c r="G42">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>91</v>
       </c>
@@ -1995,8 +2265,14 @@
       <c r="D43" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E43">
+        <v>8</v>
+      </c>
+      <c r="G43">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>93</v>
       </c>
@@ -2009,8 +2285,14 @@
       <c r="D44" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E44">
+        <v>8</v>
+      </c>
+      <c r="G44">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>95</v>
       </c>
@@ -2023,8 +2305,14 @@
       <c r="D45" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E45">
+        <v>8</v>
+      </c>
+      <c r="G45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>97</v>
       </c>
@@ -2037,8 +2325,14 @@
       <c r="D46" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E46">
+        <v>8</v>
+      </c>
+      <c r="G46">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>99</v>
       </c>
@@ -2051,8 +2345,14 @@
       <c r="D47" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E47">
+        <v>8</v>
+      </c>
+      <c r="G47">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>101</v>
       </c>
@@ -2065,8 +2365,14 @@
       <c r="D48" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E48">
+        <v>8</v>
+      </c>
+      <c r="G48">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>103</v>
       </c>
@@ -2079,8 +2385,14 @@
       <c r="D49" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E49">
+        <v>100</v>
+      </c>
+      <c r="G49">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>105</v>
       </c>
@@ -2093,8 +2405,14 @@
       <c r="D50" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E50">
+        <v>8</v>
+      </c>
+      <c r="G50">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>107</v>
       </c>
@@ -2107,8 +2425,14 @@
       <c r="D51" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E51">
+        <v>100</v>
+      </c>
+      <c r="G51">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>109</v>
       </c>
@@ -2121,8 +2445,14 @@
       <c r="D52" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E52">
+        <v>8</v>
+      </c>
+      <c r="G52">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>111</v>
       </c>
@@ -2135,8 +2465,14 @@
       <c r="D53" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E53">
+        <v>8</v>
+      </c>
+      <c r="G53">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>113</v>
       </c>
@@ -2149,8 +2485,14 @@
       <c r="D54" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E54">
+        <v>40</v>
+      </c>
+      <c r="G54">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>115</v>
       </c>
@@ -2163,8 +2505,14 @@
       <c r="D55" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E55">
+        <v>8</v>
+      </c>
+      <c r="G55">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>117</v>
       </c>
@@ -2177,8 +2525,14 @@
       <c r="D56" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E56">
+        <v>40</v>
+      </c>
+      <c r="G56">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>119</v>
       </c>
@@ -2191,8 +2545,14 @@
       <c r="D57" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E57">
+        <v>19</v>
+      </c>
+      <c r="G57">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>121</v>
       </c>
@@ -2205,8 +2565,14 @@
       <c r="D58" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E58">
+        <v>8</v>
+      </c>
+      <c r="G58">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>123</v>
       </c>
@@ -2219,8 +2585,14 @@
       <c r="D59" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E59">
+        <v>8</v>
+      </c>
+      <c r="G59">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>125</v>
       </c>
@@ -2233,8 +2605,14 @@
       <c r="D60" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E60">
+        <v>8</v>
+      </c>
+      <c r="G60">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>127</v>
       </c>
@@ -2247,8 +2625,14 @@
       <c r="D61" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E61">
+        <v>8</v>
+      </c>
+      <c r="G61">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>129</v>
       </c>
@@ -2261,8 +2645,14 @@
       <c r="D62" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E62">
+        <v>8</v>
+      </c>
+      <c r="G62">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>131</v>
       </c>
@@ -2275,8 +2665,14 @@
       <c r="D63" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E63">
+        <v>8</v>
+      </c>
+      <c r="G63">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>133</v>
       </c>
@@ -2289,8 +2685,14 @@
       <c r="D64" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E64">
+        <v>8</v>
+      </c>
+      <c r="G64">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>135</v>
       </c>
@@ -2303,8 +2705,14 @@
       <c r="D65" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E65">
+        <v>1</v>
+      </c>
+      <c r="G65">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>137</v>
       </c>
@@ -2317,8 +2725,14 @@
       <c r="D66" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E66">
+        <v>8</v>
+      </c>
+      <c r="G66">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>139</v>
       </c>
@@ -2331,8 +2745,14 @@
       <c r="D67" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E67">
+        <v>60</v>
+      </c>
+      <c r="G67">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>141</v>
       </c>
@@ -2345,8 +2765,14 @@
       <c r="D68" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E68">
+        <v>8</v>
+      </c>
+      <c r="G68">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>143</v>
       </c>
@@ -2359,8 +2785,14 @@
       <c r="D69" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E69">
+        <v>60</v>
+      </c>
+      <c r="G69">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>145</v>
       </c>
@@ -2373,8 +2805,14 @@
       <c r="D70" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E70">
+        <v>8</v>
+      </c>
+      <c r="G70">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>147</v>
       </c>
@@ -2387,8 +2825,14 @@
       <c r="D71" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E71">
+        <v>100</v>
+      </c>
+      <c r="G71">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>149</v>
       </c>
@@ -2401,8 +2845,14 @@
       <c r="D72" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E72">
+        <v>8</v>
+      </c>
+      <c r="G72">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>151</v>
       </c>
@@ -2415,8 +2865,14 @@
       <c r="D73" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E73">
+        <v>100</v>
+      </c>
+      <c r="G73">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>153</v>
       </c>
@@ -2429,8 +2885,14 @@
       <c r="D74" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E74">
+        <v>8</v>
+      </c>
+      <c r="G74">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>155</v>
       </c>
@@ -2443,8 +2905,14 @@
       <c r="D75" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E75">
+        <v>3</v>
+      </c>
+      <c r="G75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>157</v>
       </c>
@@ -2457,8 +2925,14 @@
       <c r="D76" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E76">
+        <v>100</v>
+      </c>
+      <c r="G76">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>159</v>
       </c>
@@ -2471,8 +2945,14 @@
       <c r="D77" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E77">
+        <v>8</v>
+      </c>
+      <c r="G77">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>161</v>
       </c>
@@ -2485,8 +2965,14 @@
       <c r="D78" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E78">
+        <v>8</v>
+      </c>
+      <c r="G78">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>163</v>
       </c>
@@ -2499,8 +2985,14 @@
       <c r="D79" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E79">
+        <v>8</v>
+      </c>
+      <c r="G79">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>165</v>
       </c>
@@ -2513,8 +3005,14 @@
       <c r="D80" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E80">
+        <v>8</v>
+      </c>
+      <c r="G80">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>167</v>
       </c>
@@ -2527,8 +3025,14 @@
       <c r="D81" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E81">
+        <v>8</v>
+      </c>
+      <c r="G81">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>169</v>
       </c>
@@ -2541,8 +3045,14 @@
       <c r="D82" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E82">
+        <v>8</v>
+      </c>
+      <c r="G82">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>171</v>
       </c>
@@ -2555,31 +3065,21 @@
       <c r="D83" t="s">
         <v>7</v>
       </c>
+      <c r="E83">
+        <v>8</v>
+      </c>
+      <c r="G83">
+        <v>82</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G83" xr:uid="{FC5091EF-637D-4814-8647-AFB74BF81557}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="921987c0-c4c4-4810-b0c0-7f1c7905708e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B9EE868304B98441AD61F888FD64FF20" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="328fc73772845fc8efae61a23358c59b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="921987c0-c4c4-4810-b0c0-7f1c7905708e" xmlns:ns4="6f97e022-9e66-460e-b146-2641bda6a8a8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fcacc3c0b87855621d9e2ae62a3dddf0" ns3:_="" ns4:_="">
     <xsd:import namespace="921987c0-c4c4-4810-b0c0-7f1c7905708e"/>
@@ -2814,32 +3314,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9691241-D904-4FB3-8BE4-3B637411CD98}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="6f97e022-9e66-460e-b146-2641bda6a8a8"/>
-    <ds:schemaRef ds:uri="921987c0-c4c4-4810-b0c0-7f1c7905708e"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{303332B8-B426-4220-A0AA-9F7D3C084321}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="921987c0-c4c4-4810-b0c0-7f1c7905708e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5183B734-9366-421B-B0C0-3AECEF302B29}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2856,4 +3348,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{303332B8-B426-4220-A0AA-9F7D3C084321}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9691241-D904-4FB3-8BE4-3B637411CD98}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="6f97e022-9e66-460e-b146-2641bda6a8a8"/>
+    <ds:schemaRef ds:uri="921987c0-c4c4-4810-b0c0-7f1c7905708e"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>